<commit_message>
fixed csim syn bug but struck at cosim
</commit_message>
<xml_diff>
--- a/ResourceUse.xlsx
+++ b/ResourceUse.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -384,7 +383,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B10" activeCellId="1" sqref="E8 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,16 +530,16 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D8">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E8">
-        <v>47</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more mux and s3
all good
</commit_message>
<xml_diff>
--- a/ResourceUse.xlsx
+++ b/ResourceUse.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>List</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>nufft512</t>
+  </si>
+  <si>
+    <t>s2s3</t>
+  </si>
+  <si>
+    <t>cosimbug</t>
+  </si>
+  <si>
+    <t>merge7</t>
   </si>
 </sst>
 </file>
@@ -380,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" activeCellId="1" sqref="E8 B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,6 +550,55 @@
       <c r="E8">
         <v>16</v>
       </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
all done with some bug
fut exceed100
</commit_message>
<xml_diff>
--- a/ResourceUse.xlsx
+++ b/ResourceUse.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>List</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>merge7</t>
+  </si>
+  <si>
+    <t>s3s4</t>
+  </si>
+  <si>
+    <t>final</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,28 +428,28 @@
         <v>5</v>
       </c>
       <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>28</v>
+      </c>
+      <c r="F2">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="G2">
         <v>11</v>
       </c>
-      <c r="D2">
+      <c r="H2">
         <v>13</v>
       </c>
-      <c r="E2">
+      <c r="I2">
         <v>22</v>
-      </c>
-      <c r="F2">
-        <v>12</v>
-      </c>
-      <c r="G2">
-        <v>13</v>
-      </c>
-      <c r="H2">
-        <v>17</v>
-      </c>
-      <c r="I2">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -598,6 +604,45 @@
       </c>
       <c r="I10">
         <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>